<commit_message>
update data extraction files and response variable category
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_MacMillan.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_MacMillan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A961BD6-FA20-44D9-A43F-6E810E37C480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57DD7AE-9312-4A81-B8A8-60F4AE18D70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5061,10 +5061,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AF1" sqref="AF1"/>
-      <selection pane="bottomLeft" activeCell="AU58" sqref="AU58"/>
+      <selection pane="bottomLeft" activeCell="AK45" sqref="AK45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10384,9 +10384,9 @@
         <v>110</v>
       </c>
       <c r="AH41" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK41" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI41" t="s">
         <v>148</v>
       </c>
       <c r="AM41" t="s">
@@ -10882,9 +10882,9 @@
         <v>110</v>
       </c>
       <c r="AH45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK45" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI45" t="s">
         <v>148</v>
       </c>
       <c r="AL45" t="s">
@@ -13370,15 +13370,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -13492,30 +13483,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2C7FA93-5CE6-4EAF-BCC9-E36208EBEE56}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13529,4 +13521,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>